<commit_message>
se actualiza documento de proyecto
</commit_message>
<xml_diff>
--- a/Seguimientoproyecto/Fase 3 - Seguimiento y Control/Cronograma de proyecto.xlsx
+++ b/Seguimientoproyecto/Fase 3 - Seguimiento y Control/Cronograma de proyecto.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian\Desktop\Bootcamp\Retos\0ProyectoFinal\Proyecto-EnerViva\Seguimientoproyecto\Fase 3 - Seguimiento y Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C5C399-BC5F-494D-A6D4-C21E97C113CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E89EE86-F794-4310-9CA8-0DBE9964D485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="0" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="52">
   <si>
     <t>SEGUNDO TRIMESTRE Q2</t>
   </si>
@@ -1428,67 +1428,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1510,14 +1450,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="18" xfId="42" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="25" fillId="0" borderId="52" xfId="42" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1566,20 +1566,6 @@
   </cellStyles>
   <dxfs count="37">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FFFF0000"/>
       </font>
@@ -1592,13 +1578,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF9933"/>
         </patternFill>
       </fill>
@@ -1651,6 +1630,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF9933"/>
         </patternFill>
       </fill>
@@ -1696,6 +1696,34 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -1720,6 +1748,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9933"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -1728,20 +1777,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1758,41 +1793,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9933"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -1817,6 +1817,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF9933"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -1835,13 +1842,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9933"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2155,7 +2155,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:BS37"/>
+  <dimension ref="A2:AC37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="4" ySplit="12" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
@@ -2189,35 +2189,35 @@
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="55"/>
+      <c r="D3" s="76"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="C4" s="56"/>
-      <c r="D4" s="57"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="78"/>
       <c r="E4" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="C5" s="56"/>
-      <c r="D5" s="57"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="78"/>
       <c r="E5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="C6" s="56"/>
-      <c r="D6" s="57"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="78"/>
       <c r="E6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="58"/>
-      <c r="D7" s="59"/>
+      <c r="C7" s="79"/>
+      <c r="D7" s="80"/>
       <c r="E7" t="s">
         <v>42</v>
       </c>
@@ -2226,60 +2226,60 @@
       <c r="C8" s="52"/>
     </row>
     <row r="9" spans="1:29" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="67" t="s">
+      <c r="C9" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="68"/>
-      <c r="E9" s="85"/>
-      <c r="F9" s="70" t="s">
+      <c r="D9" s="84"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="G9" s="69"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="69"/>
-      <c r="J9" s="69"/>
-      <c r="K9" s="69"/>
-      <c r="L9" s="69"/>
-      <c r="M9" s="69"/>
-      <c r="N9" s="69"/>
-      <c r="O9" s="69"/>
-      <c r="P9" s="69"/>
-      <c r="Q9" s="71"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="86"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="86"/>
+      <c r="M9" s="86"/>
+      <c r="N9" s="86"/>
+      <c r="O9" s="86"/>
+      <c r="P9" s="86"/>
+      <c r="Q9" s="87"/>
       <c r="R9" s="51"/>
     </row>
     <row r="10" spans="1:29" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="61" t="s">
+      <c r="C10" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="61" t="s">
+      <c r="D10" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="66" t="s">
+      <c r="E10" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="63" t="s">
+      <c r="F10" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="61" t="s">
+      <c r="G10" s="70"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="70"/>
+      <c r="J10" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="K10" s="61"/>
-      <c r="L10" s="61"/>
-      <c r="M10" s="61"/>
-      <c r="N10" s="61" t="s">
+      <c r="K10" s="70"/>
+      <c r="L10" s="70"/>
+      <c r="M10" s="70"/>
+      <c r="N10" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="O10" s="61"/>
-      <c r="P10" s="61"/>
-      <c r="Q10" s="62"/>
-      <c r="R10" s="73" t="s">
+      <c r="O10" s="70"/>
+      <c r="P10" s="70"/>
+      <c r="Q10" s="74"/>
+      <c r="R10" s="54" t="s">
         <v>21</v>
       </c>
       <c r="S10" s="15"/>
@@ -2296,10 +2296,10 @@
     </row>
     <row r="11" spans="1:29" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="64"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="74"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="73"/>
       <c r="F11" s="25">
         <v>1</v>
       </c>
@@ -2336,7 +2336,7 @@
       <c r="Q11" s="21">
         <v>4</v>
       </c>
-      <c r="R11" s="77">
+      <c r="R11" s="57">
         <v>4</v>
       </c>
       <c r="S11" s="16"/>
@@ -2356,7 +2356,7 @@
       <c r="B12" s="23"/>
       <c r="C12" s="30"/>
       <c r="D12" s="30"/>
-      <c r="E12" s="75"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="31"/>
       <c r="G12" s="32"/>
       <c r="H12" s="32"/>
@@ -2369,7 +2369,7 @@
       <c r="O12" s="32"/>
       <c r="P12" s="32"/>
       <c r="Q12" s="33"/>
-      <c r="R12" s="78"/>
+      <c r="R12" s="58"/>
       <c r="S12" s="17"/>
       <c r="T12" s="4"/>
       <c r="U12" s="4"/>
@@ -2384,7 +2384,7 @@
     </row>
     <row r="13" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="35"/>
-      <c r="B13" s="72" t="s">
+      <c r="B13" s="81" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="36" t="s">
@@ -2393,7 +2393,7 @@
       <c r="D13" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="76" t="s">
+      <c r="E13" s="56" t="s">
         <v>24</v>
       </c>
       <c r="F13" s="39"/>
@@ -2410,7 +2410,7 @@
       <c r="O13" s="38"/>
       <c r="P13" s="38"/>
       <c r="Q13" s="40"/>
-      <c r="R13" s="79" t="str">
+      <c r="R13" s="59" t="str">
         <f>IF(COUNTIF(F13:Q13,1)&gt;0,"Completado","Por Completar")</f>
         <v>Completado</v>
       </c>
@@ -2428,7 +2428,7 @@
     </row>
     <row r="14" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="41"/>
-      <c r="B14" s="60"/>
+      <c r="B14" s="82"/>
       <c r="C14" s="22" t="s">
         <v>25</v>
       </c>
@@ -2452,7 +2452,7 @@
       <c r="O14" s="27"/>
       <c r="P14" s="27"/>
       <c r="Q14" s="28"/>
-      <c r="R14" s="79" t="str">
+      <c r="R14" s="59" t="str">
         <f t="shared" ref="R14:R26" si="0">IF(COUNTIF(F14:Q14,1)&gt;0,"Completado","Por Completar")</f>
         <v>Completado</v>
       </c>
@@ -2470,7 +2470,7 @@
     </row>
     <row r="15" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="41"/>
-      <c r="B15" s="60"/>
+      <c r="B15" s="82"/>
       <c r="C15" s="22" t="s">
         <v>50</v>
       </c>
@@ -2494,7 +2494,7 @@
       <c r="O15" s="27"/>
       <c r="P15" s="27"/>
       <c r="Q15" s="28"/>
-      <c r="R15" s="79" t="str">
+      <c r="R15" s="59" t="str">
         <f t="shared" si="0"/>
         <v>Completado</v>
       </c>
@@ -2512,7 +2512,7 @@
     </row>
     <row r="16" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="41"/>
-      <c r="B16" s="60"/>
+      <c r="B16" s="82"/>
       <c r="C16" s="22" t="s">
         <v>28</v>
       </c>
@@ -2529,16 +2529,16 @@
       <c r="J16" s="27"/>
       <c r="K16" s="27"/>
       <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="27" t="s">
-        <v>6</v>
-      </c>
+      <c r="M16" s="27">
+        <v>1</v>
+      </c>
+      <c r="N16" s="27"/>
       <c r="O16" s="27"/>
       <c r="P16" s="27"/>
       <c r="Q16" s="28"/>
-      <c r="R16" s="79" t="str">
+      <c r="R16" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>Por Completar</v>
+        <v>Completado</v>
       </c>
       <c r="S16" s="18"/>
       <c r="T16" s="9"/>
@@ -2554,7 +2554,7 @@
     </row>
     <row r="17" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="41"/>
-      <c r="B17" s="60"/>
+      <c r="B17" s="82"/>
       <c r="C17" s="22" t="s">
         <v>29</v>
       </c>
@@ -2572,15 +2572,15 @@
       <c r="K17" s="27"/>
       <c r="L17" s="27"/>
       <c r="M17" s="27"/>
-      <c r="N17" s="27" t="s">
-        <v>6</v>
+      <c r="N17" s="27">
+        <v>1</v>
       </c>
       <c r="O17" s="27"/>
       <c r="P17" s="27"/>
       <c r="Q17" s="28"/>
-      <c r="R17" s="79" t="str">
+      <c r="R17" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>Por Completar</v>
+        <v>Completado</v>
       </c>
       <c r="S17" s="18"/>
       <c r="T17" s="9"/>
@@ -2596,7 +2596,7 @@
     </row>
     <row r="18" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="41"/>
-      <c r="B18" s="60"/>
+      <c r="B18" s="82"/>
       <c r="C18" s="22" t="s">
         <v>30</v>
       </c>
@@ -2614,15 +2614,15 @@
       <c r="K18" s="27"/>
       <c r="L18" s="27"/>
       <c r="M18" s="27"/>
-      <c r="N18" s="27" t="s">
-        <v>6</v>
+      <c r="N18" s="27">
+        <v>1</v>
       </c>
       <c r="O18" s="27"/>
       <c r="P18" s="27"/>
       <c r="Q18" s="28"/>
-      <c r="R18" s="79" t="str">
+      <c r="R18" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>Por Completar</v>
+        <v>Completado</v>
       </c>
       <c r="S18" s="18"/>
       <c r="T18" s="9"/>
@@ -2638,8 +2638,8 @@
     </row>
     <row r="19" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="41"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="84" t="s">
+      <c r="B19" s="82"/>
+      <c r="C19" s="64" t="s">
         <v>31</v>
       </c>
       <c r="D19" s="5" t="s">
@@ -2656,15 +2656,15 @@
       <c r="K19" s="27"/>
       <c r="L19" s="27"/>
       <c r="M19" s="27"/>
-      <c r="N19" s="27" t="s">
-        <v>6</v>
+      <c r="N19" s="27">
+        <v>1</v>
       </c>
       <c r="O19" s="27"/>
       <c r="P19" s="27"/>
       <c r="Q19" s="28"/>
-      <c r="R19" s="79" t="str">
+      <c r="R19" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>Por Completar</v>
+        <v>Completado</v>
       </c>
       <c r="S19" s="18"/>
       <c r="T19" s="9"/>
@@ -2680,7 +2680,7 @@
     </row>
     <row r="20" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="41"/>
-      <c r="B20" s="60"/>
+      <c r="B20" s="82"/>
       <c r="C20" s="22" t="s">
         <v>32</v>
       </c>
@@ -2698,15 +2698,15 @@
       <c r="K20" s="27"/>
       <c r="L20" s="27"/>
       <c r="M20" s="27"/>
-      <c r="N20" s="27" t="s">
-        <v>6</v>
+      <c r="N20" s="27">
+        <v>1</v>
       </c>
       <c r="O20" s="27"/>
       <c r="P20" s="27"/>
       <c r="Q20" s="28"/>
-      <c r="R20" s="79" t="str">
+      <c r="R20" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>Por Completar</v>
+        <v>Completado</v>
       </c>
       <c r="S20" s="18"/>
       <c r="T20" s="9"/>
@@ -2722,7 +2722,7 @@
     </row>
     <row r="21" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="41"/>
-      <c r="B21" s="60"/>
+      <c r="B21" s="82"/>
       <c r="C21" s="22" t="s">
         <v>36</v>
       </c>
@@ -2740,15 +2740,15 @@
       <c r="K21" s="27"/>
       <c r="L21" s="27"/>
       <c r="M21" s="27"/>
-      <c r="N21" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="O21" s="27"/>
+      <c r="N21" s="27"/>
+      <c r="O21" s="27">
+        <v>1</v>
+      </c>
       <c r="P21" s="27"/>
       <c r="Q21" s="28"/>
-      <c r="R21" s="79" t="str">
+      <c r="R21" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>Por Completar</v>
+        <v>Completado</v>
       </c>
       <c r="S21" s="18"/>
       <c r="T21" s="9"/>
@@ -2764,7 +2764,7 @@
     </row>
     <row r="22" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="41"/>
-      <c r="B22" s="60"/>
+      <c r="B22" s="82"/>
       <c r="C22" s="22" t="s">
         <v>37</v>
       </c>
@@ -2782,15 +2782,13 @@
       <c r="K22" s="27"/>
       <c r="L22" s="27"/>
       <c r="M22" s="27"/>
-      <c r="N22" s="27" t="s">
-        <v>6</v>
-      </c>
+      <c r="N22" s="27"/>
       <c r="O22" s="27" t="s">
         <v>6</v>
       </c>
       <c r="P22" s="27"/>
       <c r="Q22" s="28"/>
-      <c r="R22" s="79" t="str">
+      <c r="R22" s="59" t="str">
         <f t="shared" si="0"/>
         <v>Por Completar</v>
       </c>
@@ -2808,7 +2806,7 @@
     </row>
     <row r="23" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="41"/>
-      <c r="B23" s="60"/>
+      <c r="B23" s="82"/>
       <c r="C23" s="22" t="s">
         <v>38</v>
       </c>
@@ -2826,15 +2824,13 @@
       <c r="K23" s="27"/>
       <c r="L23" s="27"/>
       <c r="M23" s="27"/>
-      <c r="N23" s="27" t="s">
-        <v>6</v>
-      </c>
+      <c r="N23" s="27"/>
       <c r="O23" s="27" t="s">
         <v>6</v>
       </c>
       <c r="P23" s="27"/>
       <c r="Q23" s="28"/>
-      <c r="R23" s="79" t="str">
+      <c r="R23" s="59" t="str">
         <f t="shared" si="0"/>
         <v>Por Completar</v>
       </c>
@@ -2852,7 +2848,7 @@
     </row>
     <row r="24" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="41"/>
-      <c r="B24" s="60"/>
+      <c r="B24" s="82"/>
       <c r="C24" s="22" t="s">
         <v>47</v>
       </c>
@@ -2870,15 +2866,13 @@
       <c r="K24" s="27"/>
       <c r="L24" s="27"/>
       <c r="M24" s="27"/>
-      <c r="N24" s="27" t="s">
-        <v>6</v>
-      </c>
+      <c r="N24" s="27"/>
       <c r="O24" s="27" t="s">
         <v>6</v>
       </c>
       <c r="P24" s="27"/>
       <c r="Q24" s="28"/>
-      <c r="R24" s="79" t="str">
+      <c r="R24" s="59" t="str">
         <f t="shared" si="0"/>
         <v>Por Completar</v>
       </c>
@@ -2896,7 +2890,7 @@
     </row>
     <row r="25" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="41"/>
-      <c r="B25" s="60"/>
+      <c r="B25" s="82"/>
       <c r="C25" s="22" t="s">
         <v>48</v>
       </c>
@@ -2920,7 +2914,7 @@
       </c>
       <c r="P25" s="27"/>
       <c r="Q25" s="28"/>
-      <c r="R25" s="79" t="str">
+      <c r="R25" s="59" t="str">
         <f t="shared" si="0"/>
         <v>Por Completar</v>
       </c>
@@ -2962,7 +2956,7 @@
         <v>6</v>
       </c>
       <c r="Q26" s="28"/>
-      <c r="R26" s="79" t="str">
+      <c r="R26" s="59" t="str">
         <f t="shared" si="0"/>
         <v>Por Completar</v>
       </c>
@@ -2996,7 +2990,7 @@
       <c r="O27" s="48"/>
       <c r="P27" s="48"/>
       <c r="Q27" s="49"/>
-      <c r="R27" s="80"/>
+      <c r="R27" s="60"/>
       <c r="S27" s="20"/>
       <c r="T27" s="10"/>
       <c r="U27" s="10"/>
@@ -3011,7 +3005,7 @@
     </row>
     <row r="28" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="29"/>
-      <c r="E28" s="86" t="s">
+      <c r="E28" s="66" t="s">
         <v>19</v>
       </c>
       <c r="F28" s="34">
@@ -3044,15 +3038,15 @@
       </c>
       <c r="M28" s="34">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N28" s="34">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O28" s="34">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P28" s="34">
         <f t="shared" si="1"/>
@@ -3062,14 +3056,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R28" s="81">
+      <c r="R28" s="61">
         <f>COUNTIF(R13:R26,"Completado")</f>
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="29"/>
-      <c r="E29" s="87" t="s">
+      <c r="E29" s="67" t="s">
         <v>20</v>
       </c>
       <c r="F29" s="34">
@@ -3102,15 +3096,15 @@
       </c>
       <c r="M29" s="34">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N29" s="34">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="O29" s="34">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P29" s="34">
         <f t="shared" si="2"/>
@@ -3120,67 +3114,67 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R29" s="81">
+      <c r="R29" s="61">
         <f>COUNTA(C13:C26)</f>
         <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:29" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B30" s="29"/>
-      <c r="E30" s="87" t="s">
+      <c r="E30" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="F30" s="82">
+      <c r="F30" s="62">
         <f>IFERROR(F28/F29,0)</f>
         <v>0</v>
       </c>
-      <c r="G30" s="82">
+      <c r="G30" s="62">
         <f t="shared" ref="G30:Q30" si="3">IFERROR(G28/G29,0)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="82">
+      <c r="H30" s="62">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I30" s="82">
+      <c r="I30" s="62">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J30" s="82">
+      <c r="J30" s="62">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="K30" s="82">
+      <c r="K30" s="62">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="L30" s="82">
+      <c r="L30" s="62">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M30" s="82">
+      <c r="M30" s="62">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="N30" s="62">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="O30" s="62">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="P30" s="62">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N30" s="82">
+      <c r="Q30" s="62">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O30" s="82">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P30" s="82">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q30" s="82">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="R30" s="83">
+      <c r="R30" s="63">
         <f>+R28/R29</f>
-        <v>0.21428571428571427</v>
+        <v>0.6428571428571429</v>
       </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.25">
@@ -3209,92 +3203,94 @@
     <sortCondition ref="C39"/>
   </sortState>
   <mergeCells count="11">
+    <mergeCell ref="C3:D7"/>
+    <mergeCell ref="B13:B25"/>
+    <mergeCell ref="J10:M10"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:Q9"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="N10:Q10"/>
     <mergeCell ref="F10:I10"/>
-    <mergeCell ref="C3:D7"/>
-    <mergeCell ref="B13:B25"/>
-    <mergeCell ref="J10:M10"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F9:Q9"/>
   </mergeCells>
-  <conditionalFormatting sqref="F13:P18 Q14:Q18 S13:Y25 F27:R27 F20:Q26">
-    <cfRule type="cellIs" dxfId="36" priority="444" operator="equal">
+  <conditionalFormatting sqref="F13:P18 Q14:Q18 F20:Q26 F27:R27 F12:Y12 S13:Y25">
+    <cfRule type="cellIs" dxfId="36" priority="497" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="498" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="499" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13:P18 Q14:Q18 F20:Q26 F27:R27 S13:Y25">
+    <cfRule type="cellIs" dxfId="33" priority="444" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q14:Q18 S13:Y25 F13:P18 F12:Y12 F27:R27 F20:Q26">
-    <cfRule type="cellIs" dxfId="35" priority="497" operator="equal">
+  <conditionalFormatting sqref="F13:Q18">
+    <cfRule type="cellIs" dxfId="32" priority="290" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="498" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="291" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="499" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="292" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19:Q19">
-    <cfRule type="cellIs" dxfId="32" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="12" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="13" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="14" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="15" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="26" priority="15" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",F19)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="16" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="20" operator="equal">
+      <formula>x</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F19:Q26 F27:R27">
+    <cfRule type="cellIs" dxfId="23" priority="17" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F19:Q26">
+    <cfRule type="cellIs" dxfId="22" priority="18" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="20" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F27:R27 F13:P18 Q14:Q18 F20:Q26">
+    <cfRule type="containsText" dxfId="20" priority="368" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",F13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F27:R27">
+    <cfRule type="cellIs" dxfId="19" priority="366" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="367" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12:Y12 F13:P18 S13:Y25 Q14:Q18 F20:Q26 F27:R27">
+    <cfRule type="cellIs" dxfId="17" priority="500" operator="equal">
       <formula>x</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F27:R27 F19:Q26">
-    <cfRule type="cellIs" dxfId="24" priority="17" operator="equal">
-      <formula>4</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F13:P18 Q14:Q18 F27:R27 F20:Q26">
-    <cfRule type="containsText" dxfId="23" priority="368" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",F13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S13:Y25 Q14:Q18 F13:P18 F12:Y12 F27:R27 F20:Q26">
-    <cfRule type="cellIs" dxfId="22" priority="500" operator="equal">
-      <formula>x</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F27:R27 F20:Q26">
-    <cfRule type="cellIs" dxfId="21" priority="366" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="367" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F13:Q18">
-    <cfRule type="cellIs" dxfId="19" priority="290" operator="equal">
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="291" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="292" operator="equal">
-      <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q13">
@@ -3321,37 +3317,35 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R13:R26">
-    <cfRule type="cellIs" dxfId="9" priority="244" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="251" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="252" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="253" operator="equal">
+      <formula>x</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="244" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="245" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="245" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="246" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="246" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="247" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="247" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="248" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="2" priority="248" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",R13)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="249" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="249" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="253" operator="equal">
-      <formula>x</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R13:R26">
-    <cfRule type="cellIs" dxfId="2" priority="250" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="250" operator="equal">
       <formula>4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="251" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="252" operator="equal">
-      <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R30">
@@ -3409,12 +3403,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3467,15 +3458,18 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F548D624-575E-49AC-B6DA-C6CE136A6B00}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F003D47D-3505-432A-90D9-3CDE5EE91D58}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3496,9 +3490,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F003D47D-3505-432A-90D9-3CDE5EE91D58}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F548D624-575E-49AC-B6DA-C6CE136A6B00}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Se modifica el archivo py para corregir el problema de las graficas
</commit_message>
<xml_diff>
--- a/Seguimientoproyecto/Fase 3 - Seguimiento y Control/Cronograma de proyecto.xlsx
+++ b/Seguimientoproyecto/Fase 3 - Seguimiento y Control/Cronograma de proyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian\Desktop\Bootcamp\Retos\0ProyectoFinal\Proyecto-EnerViva\Seguimientoproyecto\Fase 3 - Seguimiento y Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E89EE86-F794-4310-9CA8-0DBE9964D485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89BF4FEF-19C7-4DE4-97B2-6743BB6AFB27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="0" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>SEGUNDO TRIMESTRE Q2</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>JUNIO</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <t>ESTRUCTURA DE JUICIOS FUNDAMENTALES SOBRE LA ACCIÓN</t>
@@ -2161,7 +2158,7 @@
       <pane xSplit="4" ySplit="12" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="N24" sqref="N24"/>
+      <selection pane="bottomRight" activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2176,21 +2173,20 @@
     <col min="10" max="10" width="6.28515625" customWidth="1"/>
     <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="6.42578125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="4.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="17" width="4.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="16" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="4.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="36.42578125" customWidth="1" collapsed="1"/>
     <col min="19" max="29" width="3.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="53" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C3" s="75" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="76"/>
     </row>
@@ -2198,28 +2194,28 @@
       <c r="C4" s="77"/>
       <c r="D4" s="78"/>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C5" s="77"/>
       <c r="D5" s="78"/>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C6" s="77"/>
       <c r="D6" s="78"/>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="79"/>
       <c r="D7" s="80"/>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2227,7 +2223,7 @@
     </row>
     <row r="9" spans="1:29" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="83" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="84"/>
       <c r="E9" s="65"/>
@@ -2250,10 +2246,10 @@
     <row r="10" spans="1:29" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="68" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="70" t="s">
         <v>12</v>
-      </c>
-      <c r="C10" s="70" t="s">
-        <v>13</v>
       </c>
       <c r="D10" s="70" t="s">
         <v>1</v>
@@ -2280,7 +2276,7 @@
       <c r="P10" s="70"/>
       <c r="Q10" s="74"/>
       <c r="R10" s="54" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="S10" s="15"/>
       <c r="T10" s="6"/>
@@ -2385,16 +2381,16 @@
     <row r="13" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="35"/>
       <c r="B13" s="81" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="E13" s="56" t="s">
         <v>23</v>
-      </c>
-      <c r="E13" s="56" t="s">
-        <v>24</v>
       </c>
       <c r="F13" s="39"/>
       <c r="G13" s="38"/>
@@ -2430,13 +2426,13 @@
       <c r="A14" s="41"/>
       <c r="B14" s="82"/>
       <c r="C14" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="24" t="s">
         <v>26</v>
-      </c>
-      <c r="E14" s="24" t="s">
-        <v>27</v>
       </c>
       <c r="F14" s="26"/>
       <c r="G14" s="27"/>
@@ -2472,13 +2468,13 @@
       <c r="A15" s="41"/>
       <c r="B15" s="82"/>
       <c r="C15" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="24" t="s">
         <v>50</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="24" t="s">
-        <v>51</v>
       </c>
       <c r="F15" s="26"/>
       <c r="G15" s="27"/>
@@ -2514,13 +2510,13 @@
       <c r="A16" s="41"/>
       <c r="B16" s="82"/>
       <c r="C16" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F16" s="26"/>
       <c r="G16" s="27"/>
@@ -2556,13 +2552,13 @@
       <c r="A17" s="41"/>
       <c r="B17" s="82"/>
       <c r="C17" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F17" s="26"/>
       <c r="G17" s="27"/>
@@ -2598,13 +2594,13 @@
       <c r="A18" s="41"/>
       <c r="B18" s="82"/>
       <c r="C18" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="24" t="s">
         <v>34</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>35</v>
       </c>
       <c r="F18" s="26"/>
       <c r="G18" s="27"/>
@@ -2640,13 +2636,13 @@
       <c r="A19" s="41"/>
       <c r="B19" s="82"/>
       <c r="C19" s="64" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F19" s="26"/>
       <c r="G19" s="27"/>
@@ -2682,13 +2678,13 @@
       <c r="A20" s="41"/>
       <c r="B20" s="82"/>
       <c r="C20" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F20" s="26"/>
       <c r="G20" s="27"/>
@@ -2724,13 +2720,13 @@
       <c r="A21" s="41"/>
       <c r="B21" s="82"/>
       <c r="C21" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F21" s="26"/>
       <c r="G21" s="27"/>
@@ -2766,13 +2762,13 @@
       <c r="A22" s="41"/>
       <c r="B22" s="82"/>
       <c r="C22" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F22" s="26"/>
       <c r="G22" s="27"/>
@@ -2783,14 +2779,14 @@
       <c r="L22" s="27"/>
       <c r="M22" s="27"/>
       <c r="N22" s="27"/>
-      <c r="O22" s="27" t="s">
-        <v>6</v>
+      <c r="O22" s="27">
+        <v>1</v>
       </c>
       <c r="P22" s="27"/>
       <c r="Q22" s="28"/>
       <c r="R22" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>Por Completar</v>
+        <v>Completado</v>
       </c>
       <c r="S22" s="18"/>
       <c r="T22" s="9"/>
@@ -2808,13 +2804,13 @@
       <c r="A23" s="41"/>
       <c r="B23" s="82"/>
       <c r="C23" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F23" s="26"/>
       <c r="G23" s="27"/>
@@ -2825,14 +2821,14 @@
       <c r="L23" s="27"/>
       <c r="M23" s="27"/>
       <c r="N23" s="27"/>
-      <c r="O23" s="27" t="s">
-        <v>6</v>
+      <c r="O23" s="27">
+        <v>1</v>
       </c>
       <c r="P23" s="27"/>
       <c r="Q23" s="28"/>
       <c r="R23" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>Por Completar</v>
+        <v>Completado</v>
       </c>
       <c r="S23" s="18"/>
       <c r="T23" s="9"/>
@@ -2850,13 +2846,13 @@
       <c r="A24" s="41"/>
       <c r="B24" s="82"/>
       <c r="C24" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F24" s="26"/>
       <c r="G24" s="27"/>
@@ -2867,14 +2863,14 @@
       <c r="L24" s="27"/>
       <c r="M24" s="27"/>
       <c r="N24" s="27"/>
-      <c r="O24" s="27" t="s">
-        <v>6</v>
+      <c r="O24" s="27">
+        <v>1</v>
       </c>
       <c r="P24" s="27"/>
       <c r="Q24" s="28"/>
       <c r="R24" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>Por Completar</v>
+        <v>Completado</v>
       </c>
       <c r="S24" s="18"/>
       <c r="T24" s="9"/>
@@ -2892,13 +2888,13 @@
       <c r="A25" s="41"/>
       <c r="B25" s="82"/>
       <c r="C25" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F25" s="26"/>
       <c r="G25" s="27"/>
@@ -2909,14 +2905,14 @@
       <c r="L25" s="27"/>
       <c r="M25" s="27"/>
       <c r="N25" s="27"/>
-      <c r="O25" s="27" t="s">
-        <v>6</v>
+      <c r="O25" s="27">
+        <v>1</v>
       </c>
       <c r="P25" s="27"/>
       <c r="Q25" s="28"/>
       <c r="R25" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>Por Completar</v>
+        <v>Completado</v>
       </c>
       <c r="S25" s="18"/>
       <c r="T25" s="9"/>
@@ -2934,13 +2930,13 @@
       <c r="A26" s="41"/>
       <c r="B26" s="50"/>
       <c r="C26" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F26" s="26"/>
       <c r="G26" s="27"/>
@@ -2952,13 +2948,13 @@
       <c r="M26" s="27"/>
       <c r="N26" s="27"/>
       <c r="O26" s="27"/>
-      <c r="P26" s="27" t="s">
-        <v>6</v>
+      <c r="P26" s="27">
+        <v>1</v>
       </c>
       <c r="Q26" s="28"/>
       <c r="R26" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>Por Completar</v>
+        <v>Completado</v>
       </c>
       <c r="S26" s="19"/>
       <c r="T26" s="5"/>
@@ -3006,7 +3002,7 @@
     <row r="28" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="29"/>
       <c r="E28" s="66" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F28" s="34">
         <f>COUNTIF(F13:F26,1)</f>
@@ -3046,11 +3042,11 @@
       </c>
       <c r="O28" s="34">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P28" s="34">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q28" s="34">
         <f t="shared" si="1"/>
@@ -3058,13 +3054,13 @@
       </c>
       <c r="R28" s="61">
         <f>COUNTIF(R13:R26,"Completado")</f>
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="29"/>
       <c r="E29" s="67" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F29" s="34">
         <f>COUNTA(F13:F26)</f>
@@ -3122,7 +3118,7 @@
     <row r="30" spans="1:29" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B30" s="29"/>
       <c r="E30" s="67" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F30" s="62">
         <f>IFERROR(F28/F29,0)</f>
@@ -3162,11 +3158,11 @@
       </c>
       <c r="O30" s="62">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="P30" s="62">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q30" s="62">
         <f t="shared" si="3"/>
@@ -3174,7 +3170,7 @@
       </c>
       <c r="R30" s="63">
         <f>+R28/R29</f>
-        <v>0.6428571428571429</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.25">
@@ -3374,27 +3370,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se modifica la presentacion final
</commit_message>
<xml_diff>
--- a/Seguimientoproyecto/Fase 3 - Seguimiento y Control/Cronograma de proyecto.xlsx
+++ b/Seguimientoproyecto/Fase 3 - Seguimiento y Control/Cronograma de proyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian\Desktop\Bootcamp\Retos\0ProyectoFinal\Proyecto-EnerViva\Seguimientoproyecto\Fase 3 - Seguimiento y Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89BF4FEF-19C7-4DE4-97B2-6743BB6AFB27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398C816A-0698-4996-B2A5-07D751EE62B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="0" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1455,15 +1455,54 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1474,45 +1513,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2154,11 +2154,11 @@
   </sheetPr>
   <dimension ref="A2:AC37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="4" ySplit="12" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="P26" sqref="P26"/>
+      <selection pane="bottomRight" activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2185,35 +2185,35 @@
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="76"/>
+      <c r="D3" s="69"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="C4" s="77"/>
-      <c r="D4" s="78"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="71"/>
       <c r="E4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="C5" s="77"/>
-      <c r="D5" s="78"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="71"/>
       <c r="E5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="C6" s="77"/>
-      <c r="D6" s="78"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="71"/>
       <c r="E6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="79"/>
-      <c r="D7" s="80"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="73"/>
       <c r="E7" t="s">
         <v>41</v>
       </c>
@@ -2222,59 +2222,59 @@
       <c r="C8" s="52"/>
     </row>
     <row r="9" spans="1:29" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="83" t="s">
+      <c r="C9" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="84"/>
+      <c r="D9" s="78"/>
       <c r="E9" s="65"/>
-      <c r="F9" s="85" t="s">
+      <c r="F9" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="G9" s="86"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="86"/>
-      <c r="K9" s="86"/>
-      <c r="L9" s="86"/>
-      <c r="M9" s="86"/>
-      <c r="N9" s="86"/>
-      <c r="O9" s="86"/>
-      <c r="P9" s="86"/>
-      <c r="Q9" s="87"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="80"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="80"/>
+      <c r="L9" s="80"/>
+      <c r="M9" s="80"/>
+      <c r="N9" s="80"/>
+      <c r="O9" s="80"/>
+      <c r="P9" s="80"/>
+      <c r="Q9" s="81"/>
       <c r="R9" s="51"/>
     </row>
     <row r="10" spans="1:29" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="70" t="s">
+      <c r="C10" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="70" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="72" t="s">
+      <c r="D10" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="68" t="s">
+      <c r="F10" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="70"/>
-      <c r="H10" s="70"/>
-      <c r="I10" s="70"/>
-      <c r="J10" s="70" t="s">
+      <c r="G10" s="76"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="K10" s="70"/>
-      <c r="L10" s="70"/>
-      <c r="M10" s="70"/>
-      <c r="N10" s="70" t="s">
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="O10" s="70"/>
-      <c r="P10" s="70"/>
-      <c r="Q10" s="74"/>
+      <c r="O10" s="76"/>
+      <c r="P10" s="76"/>
+      <c r="Q10" s="87"/>
       <c r="R10" s="54" t="s">
         <v>20</v>
       </c>
@@ -2292,10 +2292,10 @@
     </row>
     <row r="11" spans="1:29" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="73"/>
+      <c r="B11" s="83"/>
+      <c r="C11" s="84"/>
+      <c r="D11" s="84"/>
+      <c r="E11" s="86"/>
       <c r="F11" s="25">
         <v>1</v>
       </c>
@@ -2380,7 +2380,7 @@
     </row>
     <row r="13" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="35"/>
-      <c r="B13" s="81" t="s">
+      <c r="B13" s="74" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="36" t="s">
@@ -2424,7 +2424,7 @@
     </row>
     <row r="14" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="41"/>
-      <c r="B14" s="82"/>
+      <c r="B14" s="75"/>
       <c r="C14" s="22" t="s">
         <v>24</v>
       </c>
@@ -2466,7 +2466,7 @@
     </row>
     <row r="15" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="41"/>
-      <c r="B15" s="82"/>
+      <c r="B15" s="75"/>
       <c r="C15" s="22" t="s">
         <v>49</v>
       </c>
@@ -2508,7 +2508,7 @@
     </row>
     <row r="16" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="41"/>
-      <c r="B16" s="82"/>
+      <c r="B16" s="75"/>
       <c r="C16" s="22" t="s">
         <v>27</v>
       </c>
@@ -2550,7 +2550,7 @@
     </row>
     <row r="17" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="41"/>
-      <c r="B17" s="82"/>
+      <c r="B17" s="75"/>
       <c r="C17" s="22" t="s">
         <v>28</v>
       </c>
@@ -2592,7 +2592,7 @@
     </row>
     <row r="18" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="41"/>
-      <c r="B18" s="82"/>
+      <c r="B18" s="75"/>
       <c r="C18" s="22" t="s">
         <v>29</v>
       </c>
@@ -2634,7 +2634,7 @@
     </row>
     <row r="19" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="41"/>
-      <c r="B19" s="82"/>
+      <c r="B19" s="75"/>
       <c r="C19" s="64" t="s">
         <v>30</v>
       </c>
@@ -2676,7 +2676,7 @@
     </row>
     <row r="20" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="41"/>
-      <c r="B20" s="82"/>
+      <c r="B20" s="75"/>
       <c r="C20" s="22" t="s">
         <v>31</v>
       </c>
@@ -2718,7 +2718,7 @@
     </row>
     <row r="21" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="41"/>
-      <c r="B21" s="82"/>
+      <c r="B21" s="75"/>
       <c r="C21" s="22" t="s">
         <v>35</v>
       </c>
@@ -2758,9 +2758,9 @@
       <c r="AB21" s="3"/>
       <c r="AC21" s="3"/>
     </row>
-    <row r="22" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="41"/>
-      <c r="B22" s="82"/>
+      <c r="B22" s="75"/>
       <c r="C22" s="22" t="s">
         <v>36</v>
       </c>
@@ -2802,7 +2802,7 @@
     </row>
     <row r="23" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="41"/>
-      <c r="B23" s="82"/>
+      <c r="B23" s="75"/>
       <c r="C23" s="22" t="s">
         <v>37</v>
       </c>
@@ -2844,7 +2844,7 @@
     </row>
     <row r="24" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="41"/>
-      <c r="B24" s="82"/>
+      <c r="B24" s="75"/>
       <c r="C24" s="22" t="s">
         <v>46</v>
       </c>
@@ -2886,7 +2886,7 @@
     </row>
     <row r="25" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="41"/>
-      <c r="B25" s="82"/>
+      <c r="B25" s="75"/>
       <c r="C25" s="22" t="s">
         <v>47</v>
       </c>
@@ -3399,9 +3399,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3454,18 +3457,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F003D47D-3505-432A-90D9-3CDE5EE91D58}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F548D624-575E-49AC-B6DA-C6CE136A6B00}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3486,9 +3486,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F548D624-575E-49AC-B6DA-C6CE136A6B00}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F003D47D-3505-432A-90D9-3CDE5EE91D58}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>